<commit_message>
Update YOY Expense & Profitability Analysis data from Excel file
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACA81E-29A9-DD4D-92A1-8C3321377C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC88F89-7A83-4B43-8C17-61C7D40D276F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="3940" yWindow="760" windowWidth="25800" windowHeight="17940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="123">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Revenue Proportional</t>
   </si>
   <si>
-    <t>% of visits/revenue</t>
-  </si>
-  <si>
     <t>SUPPLY_PER_VISIT</t>
   </si>
   <si>
@@ -371,18 +368,6 @@
     <t>Value_2025_Jan_June</t>
   </si>
   <si>
-    <t>Visits to Goal</t>
-  </si>
-  <si>
-    <t>VISITS_TO_GOAL</t>
-  </si>
-  <si>
-    <t>July 2025 End of Month Visit Status</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_JULY</t>
-  </si>
-  <si>
     <t>VISIT_STATUS_AUGUST</t>
   </si>
   <si>
@@ -417,17 +402,21 @@
   </si>
   <si>
     <t>Private Visit Count</t>
+  </si>
+  <si>
+    <t>AFC / RCM Payments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -439,6 +428,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -462,13 +458,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,10 +835,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -861,17 +860,18 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3">
-        <v>729392</v>
-      </c>
-      <c r="F2" s="3">
-        <v>779143</v>
-      </c>
-      <c r="G2">
-        <v>6.8000000000000005E-2</v>
+      <c r="E2" s="6">
+        <v>896645</v>
+      </c>
+      <c r="F2" s="6">
+        <v>788324</v>
+      </c>
+      <c r="G2" s="5">
+        <f>(F2-E2)/E2</f>
+        <v>-0.12080700834778535</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -887,17 +887,18 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3">
-        <v>453952</v>
-      </c>
-      <c r="F3" s="3">
-        <v>674419</v>
-      </c>
-      <c r="G3">
-        <v>0.48599999999999999</v>
+      <c r="E3" s="6">
+        <v>689185</v>
+      </c>
+      <c r="F3" s="6">
+        <v>993263</v>
+      </c>
+      <c r="G3" s="5">
+        <f>(F3-E3)/E3</f>
+        <v>0.44121389757467155</v>
       </c>
       <c r="H3">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -914,24 +915,25 @@
         <v>14</v>
       </c>
       <c r="E4" s="3">
-        <v>4339</v>
+        <v>5438</v>
       </c>
       <c r="F4" s="3">
-        <v>4914</v>
-      </c>
-      <c r="G4">
-        <v>0.13300000000000001</v>
+        <v>6915</v>
+      </c>
+      <c r="G4" s="5">
+        <f>(F4-E4)/E4</f>
+        <v>0.27160720853254872</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -940,17 +942,17 @@
         <v>14</v>
       </c>
       <c r="E5" s="3">
-        <v>5036</v>
+        <v>4362</v>
       </c>
       <c r="F5" s="3">
-        <v>6117</v>
+        <v>5294</v>
       </c>
       <c r="G5" s="5">
-        <f>(F5-E5)/F5</f>
-        <v>0.1767206146803989</v>
+        <f>(F5-E5)/E5</f>
+        <v>0.21366345712975698</v>
       </c>
       <c r="H5">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -966,17 +968,18 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3">
-        <v>198222</v>
-      </c>
-      <c r="F6" s="3">
-        <v>192148</v>
-      </c>
-      <c r="G6">
-        <v>-3.1E-2</v>
+      <c r="E6" s="7">
+        <v>225699.18</v>
+      </c>
+      <c r="F6" s="7">
+        <v>159221.91</v>
+      </c>
+      <c r="G6" s="5">
+        <f>(F6-E6)/E6</f>
+        <v>-0.29453926239342115</v>
       </c>
       <c r="H6">
-        <v>-3</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -992,14 +995,15 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3">
-        <v>401969</v>
-      </c>
-      <c r="F7" s="3">
-        <v>439572</v>
-      </c>
-      <c r="G7">
-        <v>9.4E-2</v>
+      <c r="E7" s="7">
+        <v>680901.52</v>
+      </c>
+      <c r="F7" s="7">
+        <v>620612.53</v>
+      </c>
+      <c r="G7" s="5">
+        <f>(F7-E7)/E7</f>
+        <v>-8.8542892370103668E-2</v>
       </c>
       <c r="H7">
         <v>9</v>
@@ -1018,17 +1022,18 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3">
-        <v>62401</v>
-      </c>
-      <c r="F8" s="3">
-        <v>47594</v>
-      </c>
-      <c r="G8">
-        <v>-0.23699999999999999</v>
+      <c r="E8" s="7">
+        <v>56459.1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>64665.48</v>
+      </c>
+      <c r="G8" s="5">
+        <f>(F8-E8)/E8</f>
+        <v>0.14535088232012208</v>
       </c>
       <c r="H8">
-        <v>-24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1042,27 +1047,28 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3">
-        <v>33533</v>
-      </c>
-      <c r="F9" s="3">
-        <v>48384</v>
-      </c>
-      <c r="G9">
-        <v>0.443</v>
+        <v>122</v>
+      </c>
+      <c r="E9" s="7">
+        <v>109088.61</v>
+      </c>
+      <c r="F9" s="7">
+        <v>133508.6</v>
+      </c>
+      <c r="G9" s="5">
+        <f>(F9-E9)/E9</f>
+        <v>0.22385462606957779</v>
       </c>
       <c r="H9">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1070,25 +1076,26 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>0.33300000000000002</v>
+      <c r="E10" s="7">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="F10" s="7">
+        <v>8.68</v>
+      </c>
+      <c r="G10" s="5">
+        <f>(F10-E10)/E10</f>
+        <v>-0.46846295162278012</v>
       </c>
       <c r="H10">
-        <v>33</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1098,25 +1105,26 @@
       </c>
       <c r="E11" s="4">
         <f>E2/E4</f>
-        <v>168.10140585388339</v>
+        <v>164.88506803972049</v>
       </c>
       <c r="F11" s="4">
         <f>F2/F4</f>
-        <v>158.55575905575907</v>
-      </c>
-      <c r="G11">
-        <v>-4.8000000000000001E-2</v>
+        <v>114.00202458423716</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" ref="G11:G12" si="0">(F11-E11)/E11</f>
+        <v>-0.3085970370781283</v>
       </c>
       <c r="H11">
-        <v>-5</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -1126,25 +1134,26 @@
       </c>
       <c r="E12" s="4">
         <f>E3/E4</f>
-        <v>104.62134132288546</v>
+        <v>126.73501287237956</v>
       </c>
       <c r="F12" s="4">
         <f>F3/F4</f>
-        <v>137.24440374440374</v>
-      </c>
-      <c r="G12">
-        <v>0.30499999999999999</v>
+        <v>143.63890093998555</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.13337977946653129</v>
       </c>
       <c r="H12">
-        <v>31</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1154,235 +1163,232 @@
       </c>
       <c r="E13" s="4">
         <f>E12-E11</f>
-        <v>-63.480064530997936</v>
+        <v>-38.150055167340938</v>
       </c>
       <c r="F13" s="4">
         <f>F12-F11</f>
-        <v>-21.311355311355328</v>
-      </c>
-      <c r="G13">
-        <v>0.97499999999999998</v>
+        <v>29.636876355748385</v>
+      </c>
+      <c r="G13" s="5">
+        <f>-1*(F13-E13)/E13</f>
+        <v>1.776850157247468</v>
       </c>
       <c r="H13">
-        <v>98</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4">
-        <f>-((E3-E2)/E12)</f>
-        <v>2632.7324474834345</v>
-      </c>
-      <c r="F14" s="4">
-        <f>-((F3-F2)/F12)</f>
-        <v>763.04750607559993</v>
+        <v>35</v>
+      </c>
+      <c r="E14" s="8">
+        <v>840</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15">
-        <v>566</v>
+        <v>37</v>
+      </c>
+      <c r="F15" s="2">
+        <f>E14*(1+$G$4)</f>
+        <v>1068.150055167341</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2">
-        <f>E15*(1+$G$4)</f>
-        <v>641.27800000000002</v>
+        <f>F15*F11</f>
+        <v>121771.26884884149</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2">
-        <f>F16*F11</f>
-        <v>101678.32005575906</v>
+        <f>F15*F12</f>
+        <v>153427.89996322177</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="2">
-        <f>F16*F12</f>
-        <v>88011.816744403739</v>
+        <f>F17-F16</f>
+        <v>31656.631114380289</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2">
-        <f>F18-F17</f>
-        <v>-13666.503311355322</v>
+        <f>31153+F18</f>
+        <v>62809.631114380289</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="2">
-        <f>(F19/$F$12)</f>
-        <v>-99.57785482318863</v>
+      <c r="E20">
+        <v>685</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2">
-        <f>31153+F19</f>
-        <v>17486.496688644678</v>
+        <f>E20*(1+$G$4)</f>
+        <v>871.05093784479584</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22">
-        <v>685</v>
+        <v>37</v>
+      </c>
+      <c r="F22" s="1">
+        <f>F21*$F$11</f>
+        <v>99301.570430305248</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="2">
-        <f>E22*(1+$G$4)</f>
-        <v>776.10500000000002</v>
+        <v>37</v>
+      </c>
+      <c r="F23" s="1">
+        <f>F21*$F$12</f>
+        <v>125116.79937477014</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="1">
-        <f>F23*$F$11</f>
-        <v>123055.91738196989</v>
+        <v>37</v>
+      </c>
+      <c r="F24" s="2">
+        <f>F23-F22</f>
+        <v>25815.228944464892</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="1">
-        <f>F23*$F$12</f>
-        <v>106516.06796805047</v>
+        <v>37</v>
+      </c>
+      <c r="F25" s="2">
+        <f>(F24/$F$12)</f>
+        <v>179.72310269382299</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1393,550 +1399,514 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="2">
-        <f>F25-F24</f>
-        <v>-16539.849413919423</v>
+        <f>F19+F24</f>
+        <v>88624.860058845181</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
         <v>35</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="2">
-        <f>(F26/$F$12)</f>
-        <v>-120.51383490085547</v>
+      <c r="E27">
+        <v>808</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="2">
-        <f>F21+F26</f>
-        <v>946.64727472525556</v>
+        <f>E27*(1+$G$4)</f>
+        <v>1027.4586244942993</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29">
-        <v>808</v>
+        <v>37</v>
+      </c>
+      <c r="F29" s="1">
+        <f>F28*$F$11</f>
+        <v>117132.36336888561</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="2">
-        <f>E29*(1+$G$4)</f>
-        <v>915.46400000000006</v>
+        <v>37</v>
+      </c>
+      <c r="F30" s="1">
+        <f>F28*$F$12</f>
+        <v>147583.02758367048</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="1">
-        <f>F30*$F$11</f>
-        <v>145152.08940822142</v>
+        <v>37</v>
+      </c>
+      <c r="F31" s="2">
+        <f>F30-F29</f>
+        <v>30450.664214784876</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="1">
-        <f>F30*$F$12</f>
-        <v>125642.31082946683</v>
+        <v>37</v>
+      </c>
+      <c r="F32" s="2">
+        <f>(F31/$F$12)</f>
+        <v>211.99455033081611</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33" s="2">
-        <f>F32-F31</f>
-        <v>-19509.778578754587</v>
+        <f>F26+F31</f>
+        <v>119075.52427363006</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
         <v>35</v>
       </c>
-      <c r="D34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="2">
-        <f>(F33/$F$12)</f>
-        <v>-142.15354540130105</v>
+      <c r="E34">
+        <v>784</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="2">
-        <f>F28+F33</f>
-        <v>-18563.131304029332</v>
+        <f>E34*(1+$G$4)</f>
+        <v>996.94005148951817</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36">
-        <v>784</v>
+        <v>37</v>
+      </c>
+      <c r="F36" s="1">
+        <f>F35*$F$11</f>
+        <v>113653.18425891871</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37" s="2">
-        <f>E36*(1+$G$4)</f>
-        <v>888.27200000000005</v>
+        <v>37</v>
+      </c>
+      <c r="F37" s="1">
+        <f>F35*$F$12</f>
+        <v>143199.37329900698</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="1">
-        <f>F37*$F$11</f>
-        <v>140840.64120797723</v>
+        <v>37</v>
+      </c>
+      <c r="F38" s="2">
+        <f>F37-F36</f>
+        <v>29546.189040088269</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="1">
-        <f>F37*$F$12</f>
-        <v>121910.36100284901</v>
+        <v>37</v>
+      </c>
+      <c r="F39" s="2">
+        <f>(F38/$F$12)</f>
+        <v>205.69768249920753</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40" s="2">
-        <f>F39-F38</f>
-        <v>-18930.28020512822</v>
+        <f>F33+F38</f>
+        <v>148621.71331371833</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" t="s">
         <v>35</v>
       </c>
-      <c r="D41" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="2">
-        <f>(F40/$F$12)</f>
-        <v>-137.93116286462879</v>
+      <c r="E41">
+        <v>830</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="2">
-        <f>F35+F40</f>
-        <v>-37493.411509157551</v>
+        <f>E41*(1+$G$4)</f>
+        <v>1055.4339830820154</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43">
-        <v>830</v>
+        <v>37</v>
+      </c>
+      <c r="F43" s="1">
+        <f>F42*$F$11</f>
+        <v>120321.61088635527</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="2">
-        <f>E43*(1+$G$4)</f>
-        <v>940.39</v>
+        <v>37</v>
+      </c>
+      <c r="F44" s="1">
+        <f>F42*$F$12</f>
+        <v>151601.377344612</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="1">
-        <f>F44*$F$11</f>
-        <v>149104.25025844527</v>
+        <v>37</v>
+      </c>
+      <c r="F45" s="2">
+        <f>F44-F43</f>
+        <v>31279.766458256738</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="1">
-        <f>F44*$F$12</f>
-        <v>129063.26483719984</v>
+        <v>37</v>
+      </c>
+      <c r="F46" s="2">
+        <f>(F45/$F$12)</f>
+        <v>217.76667917645713</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F47" s="2">
-        <f>F46-F45</f>
-        <v>-20040.985421245437</v>
+        <f>F40+F45</f>
+        <v>179901.47977197508</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" t="s">
         <v>35</v>
       </c>
-      <c r="D48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="2">
-        <f>(F47/$F$12)</f>
-        <v>-146.02406272658405</v>
+      <c r="E48">
+        <v>754</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F49" s="2">
-        <f>F42+F47</f>
-        <v>-57534.396930402989</v>
+        <f>E48*(1+$G$4)</f>
+        <v>958.79183523354175</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50">
-        <v>754</v>
+        <v>37</v>
+      </c>
+      <c r="F50" s="1">
+        <f>F49*$F$11</f>
+        <v>109304.2103714601</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="2">
-        <f>E50*(1+$G$4)</f>
-        <v>854.28200000000004</v>
+        <v>37</v>
+      </c>
+      <c r="F51" s="1">
+        <f>F49*$F$12</f>
+        <v>137719.80544317764</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="1">
-        <f>F51*$F$11</f>
-        <v>135451.33095767198</v>
+        <v>37</v>
+      </c>
+      <c r="F52" s="2">
+        <f>F51-F50</f>
+        <v>28415.595071717544</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="1">
-        <f>F51*$F$12</f>
-        <v>117245.42371957672</v>
+        <v>37</v>
+      </c>
+      <c r="F53" s="2">
+        <f>(F52/$F$12)</f>
+        <v>197.82659770969704</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F54" s="2">
-        <f>F53-F52</f>
-        <v>-18205.907238095257</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>123</v>
-      </c>
-      <c r="B55" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="2">
-        <f>(F54/$F$12)</f>
-        <v>-132.65318469378843</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" t="s">
-        <v>35</v>
-      </c>
-      <c r="D56" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="2">
-        <f>F54+F49</f>
-        <v>-75740.304168498245</v>
+        <f>F52+F47</f>
+        <v>208317.07484369262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update YOY data with new column names, preserve original cashflow data
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC88F89-7A83-4B43-8C17-61C7D40D276F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E8AE8-896A-E549-8D49-6CB034B651DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="760" windowWidth="25800" windowHeight="17940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="5000" yWindow="1520" windowWidth="25800" windowHeight="17940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -362,12 +362,6 @@
     <t>July 2025 End of Month Cash Position</t>
   </si>
   <si>
-    <t>Value_2024_Jan_June</t>
-  </si>
-  <si>
-    <t>Value_2025_Jan_June</t>
-  </si>
-  <si>
     <t>VISIT_STATUS_AUGUST</t>
   </si>
   <si>
@@ -405,6 +399,12 @@
   </si>
   <si>
     <t>AFC / RCM Payments</t>
+  </si>
+  <si>
+    <t>Value_2024_Jan_July</t>
+  </si>
+  <si>
+    <t>Value_2025_Jan_July</t>
   </si>
 </sst>
 </file>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,10 +835,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -915,25 +915,25 @@
         <v>14</v>
       </c>
       <c r="E4" s="3">
-        <v>5438</v>
+        <v>6263</v>
       </c>
       <c r="F4" s="3">
-        <v>6915</v>
+        <v>7902</v>
       </c>
       <c r="G4" s="5">
         <f>(F4-E4)/E4</f>
-        <v>0.27160720853254872</v>
+        <v>0.26169567300015967</v>
       </c>
       <c r="H4">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -942,17 +942,17 @@
         <v>14</v>
       </c>
       <c r="E5" s="3">
-        <v>4362</v>
+        <v>5036</v>
       </c>
       <c r="F5" s="3">
-        <v>5294</v>
+        <v>6117</v>
       </c>
       <c r="G5" s="5">
         <f>(F5-E5)/E5</f>
-        <v>0.21366345712975698</v>
+        <v>0.21465448768864179</v>
       </c>
       <c r="H5">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -969,17 +969,17 @@
         <v>17</v>
       </c>
       <c r="E6" s="7">
-        <v>225699.18</v>
+        <v>282396</v>
       </c>
       <c r="F6" s="7">
-        <v>159221.91</v>
+        <v>215022</v>
       </c>
       <c r="G6" s="5">
         <f>(F6-E6)/E6</f>
-        <v>-0.29453926239342115</v>
+        <v>-0.23857986657034802</v>
       </c>
       <c r="H6">
-        <v>-30</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -996,17 +996,17 @@
         <v>20</v>
       </c>
       <c r="E7" s="7">
-        <v>680901.52</v>
+        <v>313970</v>
       </c>
       <c r="F7" s="7">
-        <v>620612.53</v>
+        <v>305786</v>
       </c>
       <c r="G7" s="5">
         <f>(F7-E7)/E7</f>
-        <v>-8.8542892370103668E-2</v>
+        <v>-2.6066184667324903E-2</v>
       </c>
       <c r="H7">
-        <v>9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1023,14 +1023,14 @@
         <v>17</v>
       </c>
       <c r="E8" s="7">
-        <v>56459.1</v>
+        <v>56914</v>
       </c>
       <c r="F8" s="7">
         <v>64665.48</v>
       </c>
       <c r="G8" s="5">
         <f>(F8-E8)/E8</f>
-        <v>0.14535088232012208</v>
+        <v>0.13619636644762279</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -1047,20 +1047,20 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="7">
-        <v>109088.61</v>
+        <v>70417</v>
       </c>
       <c r="F9" s="7">
-        <v>133508.6</v>
+        <v>84980</v>
       </c>
       <c r="G9" s="5">
         <f>(F9-E9)/E9</f>
-        <v>0.22385462606957779</v>
+        <v>0.20681085533322918</v>
       </c>
       <c r="H9">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1077,17 +1077,19 @@
         <v>20</v>
       </c>
       <c r="E10" s="7">
-        <v>16.329999999999998</v>
+        <f>108025/E4</f>
+        <v>17.24812390228325</v>
       </c>
       <c r="F10" s="7">
-        <v>8.68</v>
+        <f>74590/F4</f>
+        <v>9.4393824348266264</v>
       </c>
       <c r="G10" s="5">
         <f>(F10-E10)/E10</f>
-        <v>-0.46846295162278012</v>
+        <v>-0.4527299033620073</v>
       </c>
       <c r="H10">
-        <v>-47</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1105,18 +1107,18 @@
       </c>
       <c r="E11" s="4">
         <f>E2/E4</f>
-        <v>164.88506803972049</v>
+        <v>143.1654159348555</v>
       </c>
       <c r="F11" s="4">
         <f>F2/F4</f>
-        <v>114.00202458423716</v>
+        <v>99.762591748924322</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" ref="G11:G12" si="0">(F11-E11)/E11</f>
-        <v>-0.3085970370781283</v>
+        <v>-0.30316556482943302</v>
       </c>
       <c r="H11">
-        <v>-4</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1134,18 +1136,18 @@
       </c>
       <c r="E12" s="4">
         <f>E3/E4</f>
-        <v>126.73501287237956</v>
+        <v>110.04071531215072</v>
       </c>
       <c r="F12" s="4">
         <f>F3/F4</f>
-        <v>143.63890093998555</v>
+        <v>125.6976714755758</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>0.13337977946653129</v>
+        <v>0.1422833004948327</v>
       </c>
       <c r="H12">
-        <v>-2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1163,18 +1165,18 @@
       </c>
       <c r="E13" s="4">
         <f>E12-E11</f>
-        <v>-38.150055167340938</v>
+        <v>-33.124700622704779</v>
       </c>
       <c r="F13" s="4">
         <f>F12-F11</f>
-        <v>29.636876355748385</v>
+        <v>25.93507972665148</v>
       </c>
       <c r="G13" s="5">
         <f>-1*(F13-E13)/E13</f>
-        <v>1.776850157247468</v>
+        <v>1.7829528792442793</v>
       </c>
       <c r="H13">
-        <v>177</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1209,7 +1211,7 @@
       </c>
       <c r="F15" s="2">
         <f>E14*(1+$G$4)</f>
-        <v>1068.150055167341</v>
+        <v>1059.8243653201341</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1227,7 +1229,7 @@
       </c>
       <c r="F16" s="2">
         <f>F15*F11</f>
-        <v>121771.26884884149</v>
+        <v>105730.82548299537</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1245,7 +1247,7 @@
       </c>
       <c r="F17" s="2">
         <f>F15*F12</f>
-        <v>153427.89996322177</v>
+        <v>133217.45489382086</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1263,7 +1265,7 @@
       </c>
       <c r="F18" s="2">
         <f>F17-F16</f>
-        <v>31656.631114380289</v>
+        <v>27486.629410825495</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,7 +1283,7 @@
       </c>
       <c r="F19" s="2">
         <f>31153+F18</f>
-        <v>62809.631114380289</v>
+        <v>58639.629410825495</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1316,7 +1318,7 @@
       </c>
       <c r="F21" s="2">
         <f>E20*(1+$G$4)</f>
-        <v>871.05093784479584</v>
+        <v>864.26153600510929</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1334,7 +1336,7 @@
       </c>
       <c r="F22" s="1">
         <f>F21*$F$11</f>
-        <v>99301.570430305248</v>
+        <v>86220.970780775984</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1352,7 +1354,7 @@
       </c>
       <c r="F23" s="1">
         <f>F21*$F$12</f>
-        <v>125116.79937477014</v>
+        <v>108635.66262174676</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1370,15 +1372,15 @@
       </c>
       <c r="F24" s="2">
         <f>F23-F22</f>
-        <v>25815.228944464892</v>
+        <v>22414.691840970772</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1388,7 +1390,7 @@
       </c>
       <c r="F25" s="2">
         <f>(F24/$F$12)</f>
-        <v>179.72310269382299</v>
+        <v>178.32225193866182</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1406,7 +1408,7 @@
       </c>
       <c r="F26" s="2">
         <f>F19+F24</f>
-        <v>88624.860058845181</v>
+        <v>81054.321251796267</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1441,7 +1443,7 @@
       </c>
       <c r="F28" s="2">
         <f>E27*(1+$G$4)</f>
-        <v>1027.4586244942993</v>
+        <v>1019.4501037841289</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1459,7 +1461,7 @@
       </c>
       <c r="F29" s="1">
         <f>F28*$F$11</f>
-        <v>117132.36336888561</v>
+        <v>101702.98451221459</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,7 +1479,7 @@
       </c>
       <c r="F30" s="1">
         <f>F28*$F$12</f>
-        <v>147583.02758367048</v>
+        <v>128142.5042311991</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1495,15 +1497,15 @@
       </c>
       <c r="F31" s="2">
         <f>F30-F29</f>
-        <v>30450.664214784876</v>
+        <v>26439.519718984506</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
@@ -1513,7 +1515,7 @@
       </c>
       <c r="F32" s="2">
         <f>(F31/$F$12)</f>
-        <v>211.99455033081611</v>
+        <v>210.3421599510055</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1531,7 +1533,7 @@
       </c>
       <c r="F33" s="2">
         <f>F26+F31</f>
-        <v>119075.52427363006</v>
+        <v>107493.84097078077</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,7 +1568,7 @@
       </c>
       <c r="F35" s="2">
         <f>E34*(1+$G$4)</f>
-        <v>996.94005148951817</v>
+        <v>989.16940763212517</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1584,7 +1586,7 @@
       </c>
       <c r="F36" s="1">
         <f>F35*$F$11</f>
-        <v>113653.18425891871</v>
+        <v>98682.103784129009</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1602,7 +1604,7 @@
       </c>
       <c r="F37" s="1">
         <f>F35*$F$12</f>
-        <v>143199.37329900698</v>
+        <v>124336.29123423279</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1620,15 +1622,15 @@
       </c>
       <c r="F38" s="2">
         <f>F37-F36</f>
-        <v>29546.189040088269</v>
+        <v>25654.187450103782</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
@@ -1638,7 +1640,7 @@
       </c>
       <c r="F39" s="2">
         <f>(F38/$F$12)</f>
-        <v>205.69768249920753</v>
+        <v>204.09437302176772</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1656,7 +1658,7 @@
       </c>
       <c r="F40" s="2">
         <f>F33+F38</f>
-        <v>148621.71331371833</v>
+        <v>133148.02842088457</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1691,7 +1693,7 @@
       </c>
       <c r="F42" s="2">
         <f>E41*(1+$G$4)</f>
-        <v>1055.4339830820154</v>
+        <v>1047.2074085901324</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1709,7 +1711,7 @@
       </c>
       <c r="F43" s="1">
         <f>F42*$F$11</f>
-        <v>120321.61088635527</v>
+        <v>104472.12517962637</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1727,7 +1729,7 @@
       </c>
       <c r="F44" s="1">
         <f>F42*$F$12</f>
-        <v>151601.377344612</v>
+        <v>131631.53281175156</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1745,15 +1747,15 @@
       </c>
       <c r="F45" s="2">
         <f>F44-F43</f>
-        <v>31279.766458256738</v>
+        <v>27159.407632125192</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
         <v>34</v>
@@ -1763,7 +1765,7 @@
       </c>
       <c r="F46" s="2">
         <f>(F45/$F$12)</f>
-        <v>217.76667917645713</v>
+        <v>216.06929796947361</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1781,7 +1783,7 @@
       </c>
       <c r="F47" s="2">
         <f>F40+F45</f>
-        <v>179901.47977197508</v>
+        <v>160307.43605300976</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,7 +1818,7 @@
       </c>
       <c r="F49" s="2">
         <f>E48*(1+$G$4)</f>
-        <v>958.79183523354175</v>
+        <v>951.31853744212037</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1834,7 +1836,7 @@
       </c>
       <c r="F50" s="1">
         <f>F49*$F$11</f>
-        <v>109304.2103714601</v>
+        <v>94906.00287402203</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1852,7 +1854,7 @@
       </c>
       <c r="F51" s="1">
         <f>F49*$F$12</f>
-        <v>137719.80544317764</v>
+        <v>119578.5249880249</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1870,15 +1872,15 @@
       </c>
       <c r="F52" s="2">
         <f>F51-F50</f>
-        <v>28415.595071717544</v>
+        <v>24672.522114002873</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
         <v>34</v>
@@ -1888,7 +1890,7 @@
       </c>
       <c r="F53" s="2">
         <f>(F52/$F$12)</f>
-        <v>197.82659770969704</v>
+        <v>196.28463936022052</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1906,7 +1908,7 @@
       </c>
       <c r="F54" s="2">
         <f>F52+F47</f>
-        <v>208317.07484369262</v>
+        <v>184979.95816701264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update YOY data from Excel file while preserving original cashflow data
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E8AE8-896A-E549-8D49-6CB034B651DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43015C-C2C8-AE46-9FD8-F17F1D1CFC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="1520" windowWidth="25800" windowHeight="17940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="3560" yWindow="2040" windowWidth="27480" windowHeight="17980" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -324,72 +324,6 @@
   </si>
   <si>
     <t>CASHFLOW_DECEMBER_CASH_POSITION</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_VISIT_AVG</t>
-  </si>
-  <si>
-    <t>July 2023/2024 Visit Average</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_VISIT_PROJ</t>
-  </si>
-  <si>
-    <t>July 2025 Visit Projection</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_EXPENSES</t>
-  </si>
-  <si>
-    <t>July 2025 Expected Expenses</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_REVENUE</t>
-  </si>
-  <si>
-    <t>July 2025 Expected Revenue</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_PROFIT</t>
-  </si>
-  <si>
-    <t>July 2025 Expected Profit</t>
-  </si>
-  <si>
-    <t>CASHFLOW_JULY_CASH_POSITION</t>
-  </si>
-  <si>
-    <t>July 2025 End of Month Cash Position</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_AUGUST</t>
-  </si>
-  <si>
-    <t>August 2025 End of Month Visit Status</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_SEPTEMBER</t>
-  </si>
-  <si>
-    <t>September 2025 End of Month Visit Status</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_OCTOBER</t>
-  </si>
-  <si>
-    <t>October 2025 End of Month Visit Status</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_NOVEMBER</t>
-  </si>
-  <si>
-    <t>November 2025 End of Month Visit Status</t>
-  </si>
-  <si>
-    <t>VISIT_STATUS_DECEMBER</t>
-  </si>
-  <si>
-    <t>December 2025 End of Month Visit Status</t>
   </si>
   <si>
     <t>PRIVATE_VISIT_COUNT</t>
@@ -458,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,7 +401,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,15 +735,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
@@ -835,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -930,10 +863,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1047,7 +980,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E9" s="7">
         <v>70417</v>
@@ -1181,10 +1114,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -1192,16 +1125,16 @@
       <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="8">
-        <v>840</v>
+      <c r="E14">
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
@@ -1211,15 +1144,15 @@
       </c>
       <c r="F15" s="2">
         <f>E14*(1+$G$4)</f>
-        <v>1059.8243653201341</v>
+        <v>864.26153600510929</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -1227,17 +1160,17 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="2">
-        <f>F15*F11</f>
-        <v>105730.82548299537</v>
+      <c r="F16" s="1">
+        <f>F15*$F$11</f>
+        <v>86220.970780775984</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -1245,17 +1178,17 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="2">
-        <f>F15*F12</f>
-        <v>133217.45489382086</v>
+      <c r="F17" s="1">
+        <f>F15*$F$12</f>
+        <v>108635.66262174676</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1265,15 +1198,15 @@
       </c>
       <c r="F18" s="2">
         <f>F17-F16</f>
-        <v>27486.629410825495</v>
+        <v>22414.691840970772</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1282,16 +1215,16 @@
         <v>37</v>
       </c>
       <c r="F19" s="2">
-        <f>31153+F18</f>
-        <v>58639.629410825495</v>
+        <f>250000+F18</f>
+        <v>272414.69184097077</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -1300,15 +1233,15 @@
         <v>35</v>
       </c>
       <c r="E20">
-        <v>685</v>
+        <v>808</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -1318,15 +1251,15 @@
       </c>
       <c r="F21" s="2">
         <f>E20*(1+$G$4)</f>
-        <v>864.26153600510929</v>
+        <v>1019.4501037841289</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1336,15 +1269,15 @@
       </c>
       <c r="F22" s="1">
         <f>F21*$F$11</f>
-        <v>86220.970780775984</v>
+        <v>101702.98451221459</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1354,15 +1287,15 @@
       </c>
       <c r="F23" s="1">
         <f>F21*$F$12</f>
-        <v>108635.66262174676</v>
+        <v>128142.5042311991</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -1372,15 +1305,15 @@
       </c>
       <c r="F24" s="2">
         <f>F23-F22</f>
-        <v>22414.691840970772</v>
+        <v>26439.519718984506</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1389,51 +1322,51 @@
         <v>37</v>
       </c>
       <c r="F25" s="2">
-        <f>(F24/$F$12)</f>
-        <v>178.32225193866182</v>
+        <f>F19+F24</f>
+        <v>298854.21155995526</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="2">
-        <f>F19+F24</f>
-        <v>81054.321251796267</v>
+        <v>35</v>
+      </c>
+      <c r="E26">
+        <v>784</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27">
-        <v>808</v>
+        <v>37</v>
+      </c>
+      <c r="F27" s="2">
+        <f>E26*(1+$G$4)</f>
+        <v>989.16940763212517</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
@@ -1441,17 +1374,17 @@
       <c r="D28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="2">
-        <f>E27*(1+$G$4)</f>
-        <v>1019.4501037841289</v>
+      <c r="F28" s="1">
+        <f>F27*$F$11</f>
+        <v>98682.103784129009</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -1460,16 +1393,16 @@
         <v>37</v>
       </c>
       <c r="F29" s="1">
-        <f>F28*$F$11</f>
-        <v>101702.98451221459</v>
+        <f>F27*$F$12</f>
+        <v>124336.29123423279</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -1477,17 +1410,17 @@
       <c r="D30" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="1">
-        <f>F28*$F$12</f>
-        <v>128142.5042311991</v>
+      <c r="F30" s="2">
+        <f>F29-F28</f>
+        <v>25654.187450103782</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -1496,34 +1429,33 @@
         <v>37</v>
       </c>
       <c r="F31" s="2">
-        <f>F30-F29</f>
-        <v>26439.519718984506</v>
+        <f>F25+F30</f>
+        <v>324508.39901005907</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="2">
-        <f>(F31/$F$12)</f>
-        <v>210.3421599510055</v>
+        <v>35</v>
+      </c>
+      <c r="E32">
+        <v>830</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
@@ -1532,33 +1464,34 @@
         <v>37</v>
       </c>
       <c r="F33" s="2">
-        <f>F26+F31</f>
-        <v>107493.84097078077</v>
+        <f>E32*(1+$G$4)</f>
+        <v>1047.2074085901324</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34">
-        <v>784</v>
+        <v>37</v>
+      </c>
+      <c r="F34" s="1">
+        <f>F33*$F$11</f>
+        <v>104472.12517962637</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -1566,17 +1499,17 @@
       <c r="D35" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="2">
-        <f>E34*(1+$G$4)</f>
-        <v>989.16940763212517</v>
+      <c r="F35" s="1">
+        <f>F33*$F$12</f>
+        <v>131631.53281175156</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -1584,17 +1517,17 @@
       <c r="D36" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="1">
-        <f>F35*$F$11</f>
-        <v>98682.103784129009</v>
+      <c r="F36" s="2">
+        <f>F35-F34</f>
+        <v>27159.407632125192</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
@@ -1602,35 +1535,34 @@
       <c r="D37" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="1">
-        <f>F35*$F$12</f>
-        <v>124336.29123423279</v>
+      <c r="F37" s="2">
+        <f>F31+F36</f>
+        <v>351667.80664218427</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
         <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="2">
-        <f>F37-F36</f>
-        <v>25654.187450103782</v>
+        <v>35</v>
+      </c>
+      <c r="E38">
+        <v>754</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
@@ -1639,16 +1571,16 @@
         <v>37</v>
       </c>
       <c r="F39" s="2">
-        <f>(F38/$F$12)</f>
-        <v>204.09437302176772</v>
+        <f>E38*(1+$G$4)</f>
+        <v>951.31853744212037</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1656,34 +1588,35 @@
       <c r="D40" t="s">
         <v>37</v>
       </c>
-      <c r="F40" s="2">
-        <f>F33+F38</f>
-        <v>133148.02842088457</v>
+      <c r="F40" s="1">
+        <f>F39*$F$11</f>
+        <v>94906.00287402203</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41">
-        <v>830</v>
+        <v>37</v>
+      </c>
+      <c r="F41" s="1">
+        <f>F39*$F$12</f>
+        <v>119578.5249880249</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
         <v>34</v>
@@ -1692,16 +1625,16 @@
         <v>37</v>
       </c>
       <c r="F42" s="2">
-        <f>E41*(1+$G$4)</f>
-        <v>1047.2074085901324</v>
+        <f>F41-F40</f>
+        <v>24672.522114002873</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
         <v>34</v>
@@ -1709,206 +1642,9 @@
       <c r="D43" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="1">
-        <f>F42*$F$11</f>
-        <v>104472.12517962637</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F44" s="1">
-        <f>F42*$F$12</f>
-        <v>131631.53281175156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="2">
-        <f>F44-F43</f>
-        <v>27159.407632125192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
-        <v>37</v>
-      </c>
-      <c r="F46" s="2">
-        <f>(F45/$F$12)</f>
-        <v>216.06929796947361</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="2">
-        <f>F40+F45</f>
-        <v>160307.43605300976</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" s="2">
-        <f>E48*(1+$G$4)</f>
-        <v>951.31853744212037</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" t="s">
-        <v>90</v>
-      </c>
-      <c r="C50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F50" s="1">
-        <f>F49*$F$11</f>
-        <v>94906.00287402203</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" t="s">
-        <v>37</v>
-      </c>
-      <c r="F51" s="1">
-        <f>F49*$F$12</f>
-        <v>119578.5249880249</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B52" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" t="s">
-        <v>37</v>
-      </c>
-      <c r="F52" s="2">
-        <f>F51-F50</f>
-        <v>24672.522114002873</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" t="s">
-        <v>37</v>
-      </c>
-      <c r="F53" s="2">
-        <f>(F52/$F$12)</f>
-        <v>196.28463936022052</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" t="s">
-        <v>37</v>
-      </c>
-      <c r="F54" s="2">
-        <f>F52+F47</f>
-        <v>184979.95816701264</v>
+      <c r="F43" s="2">
+        <f>F42+F37</f>
+        <v>376340.32875618711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Payroll to Revenue Ratio row to YOY Expense & Profitability Analysis table
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43015C-C2C8-AE46-9FD8-F17F1D1CFC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B9468C-8018-324A-BE19-F39372D50071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="2040" windowWidth="27480" windowHeight="17980" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="4440" yWindow="1660" windowWidth="25800" windowHeight="17980" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>Value_2025_Jan_July</t>
+  </si>
+  <si>
+    <t>PAYROLL_TO_REVENUE_RATIO</t>
+  </si>
+  <si>
+    <t>Payroll to Revenue Ratio</t>
   </si>
 </sst>
 </file>
@@ -392,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,6 +407,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,7 +807,7 @@
         <v>788324</v>
       </c>
       <c r="G2" s="5">
-        <f>(F2-E2)/E2</f>
+        <f t="shared" ref="G2:G11" si="0">(F2-E2)/E2</f>
         <v>-0.12080700834778535</v>
       </c>
       <c r="H2">
@@ -827,7 +834,7 @@
         <v>993263</v>
       </c>
       <c r="G3" s="5">
-        <f>(F3-E3)/E3</f>
+        <f t="shared" si="0"/>
         <v>0.44121389757467155</v>
       </c>
       <c r="H3">
@@ -854,7 +861,7 @@
         <v>7902</v>
       </c>
       <c r="G4" s="5">
-        <f>(F4-E4)/E4</f>
+        <f t="shared" si="0"/>
         <v>0.26169567300015967</v>
       </c>
       <c r="H4">
@@ -881,7 +888,7 @@
         <v>6117</v>
       </c>
       <c r="G5" s="5">
-        <f>(F5-E5)/E5</f>
+        <f t="shared" si="0"/>
         <v>0.21465448768864179</v>
       </c>
       <c r="H5">
@@ -908,7 +915,7 @@
         <v>215022</v>
       </c>
       <c r="G6" s="5">
-        <f>(F6-E6)/E6</f>
+        <f t="shared" si="0"/>
         <v>-0.23857986657034802</v>
       </c>
       <c r="H6">
@@ -935,7 +942,7 @@
         <v>305786</v>
       </c>
       <c r="G7" s="5">
-        <f>(F7-E7)/E7</f>
+        <f t="shared" si="0"/>
         <v>-2.6066184667324903E-2</v>
       </c>
       <c r="H7">
@@ -962,7 +969,7 @@
         <v>64665.48</v>
       </c>
       <c r="G8" s="5">
-        <f>(F8-E8)/E8</f>
+        <f t="shared" si="0"/>
         <v>0.13619636644762279</v>
       </c>
       <c r="H8">
@@ -989,7 +996,7 @@
         <v>84980</v>
       </c>
       <c r="G9" s="5">
-        <f>(F9-E9)/E9</f>
+        <f t="shared" si="0"/>
         <v>0.20681085533322918</v>
       </c>
       <c r="H9">
@@ -998,10 +1005,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1009,150 +1016,159 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.20408163265306117</v>
+      </c>
+      <c r="H10">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7">
         <f>108025/E4</f>
         <v>17.24812390228325</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="7">
         <f>74590/F4</f>
         <v>9.4393824348266264</v>
       </c>
-      <c r="G10" s="5">
-        <f>(F10-E10)/E10</f>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
         <v>-0.4527299033620073</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>-45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="4">
         <f>E2/E4</f>
         <v>143.1654159348555</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F12" s="4">
         <f>F2/F4</f>
         <v>99.762591748924322</v>
       </c>
-      <c r="G11" s="5">
-        <f t="shared" ref="G11:G12" si="0">(F11-E11)/E11</f>
+      <c r="G12" s="5">
+        <f t="shared" ref="G12:G13" si="1">(F12-E12)/E12</f>
         <v>-0.30316556482943302</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>-30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="4">
         <f>E3/E4</f>
         <v>110.04071531215072</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F13" s="4">
         <f>F3/F4</f>
         <v>125.6976714755758</v>
       </c>
-      <c r="G12" s="5">
-        <f t="shared" si="0"/>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
         <v>0.1422833004948327</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4">
-        <f>E12-E11</f>
-        <v>-33.124700622704779</v>
-      </c>
-      <c r="F13" s="4">
-        <f>F12-F11</f>
-        <v>25.93507972665148</v>
-      </c>
-      <c r="G13" s="5">
-        <f>-1*(F13-E13)/E13</f>
-        <v>1.7829528792442793</v>
-      </c>
-      <c r="H13">
-        <v>1778</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14">
-        <v>685</v>
+        <v>9</v>
+      </c>
+      <c r="E14" s="4">
+        <f>E13-E12</f>
+        <v>-33.124700622704779</v>
+      </c>
+      <c r="F14" s="4">
+        <f>F13-F12</f>
+        <v>25.93507972665148</v>
+      </c>
+      <c r="G14" s="5">
+        <f>-1*(F14-E14)/E14</f>
+        <v>1.7829528792442793</v>
+      </c>
+      <c r="H14">
+        <v>1778</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="2">
-        <f>E14*(1+$G$4)</f>
-        <v>864.26153600510929</v>
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>685</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -1160,17 +1176,17 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="1">
-        <f>F15*$F$11</f>
-        <v>86220.970780775984</v>
+      <c r="F16" s="2">
+        <f>E15*(1+$G$4)</f>
+        <v>864.26153600510929</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -1179,16 +1195,16 @@
         <v>37</v>
       </c>
       <c r="F17" s="1">
-        <f>F15*$F$12</f>
-        <v>108635.66262174676</v>
+        <f>F16*$F$12</f>
+        <v>86220.970780775984</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1196,17 +1212,17 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="2">
-        <f>F17-F16</f>
-        <v>22414.691840970772</v>
+      <c r="F18" s="1">
+        <f>F16*$F$13</f>
+        <v>108635.66262174676</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1215,51 +1231,51 @@
         <v>37</v>
       </c>
       <c r="F19" s="2">
-        <f>250000+F18</f>
-        <v>272414.69184097077</v>
+        <f>F18-F17</f>
+        <v>22414.691840970772</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20">
-        <v>808</v>
+        <v>37</v>
+      </c>
+      <c r="F20" s="2">
+        <f>250000+F19</f>
+        <v>272414.69184097077</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="2">
-        <f>E20*(1+$G$4)</f>
-        <v>1019.4501037841289</v>
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1267,17 +1283,17 @@
       <c r="D22" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="1">
-        <f>F21*$F$11</f>
-        <v>101702.98451221459</v>
+      <c r="F22" s="2">
+        <f>E21*(1+$G$4)</f>
+        <v>1019.4501037841289</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1286,16 +1302,16 @@
         <v>37</v>
       </c>
       <c r="F23" s="1">
-        <f>F21*$F$12</f>
-        <v>128142.5042311991</v>
+        <f>F22*$F$12</f>
+        <v>101702.98451221459</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -1303,17 +1319,17 @@
       <c r="D24" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="2">
-        <f>F23-F22</f>
-        <v>26439.519718984506</v>
+      <c r="F24" s="1">
+        <f>F22*$F$13</f>
+        <v>128142.5042311991</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1322,51 +1338,51 @@
         <v>37</v>
       </c>
       <c r="F25" s="2">
-        <f>F19+F24</f>
-        <v>298854.21155995526</v>
+        <f>F24-F23</f>
+        <v>26439.519718984506</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26">
-        <v>784</v>
+        <v>37</v>
+      </c>
+      <c r="F26" s="2">
+        <f>F20+F25</f>
+        <v>298854.21155995526</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="2">
-        <f>E26*(1+$G$4)</f>
-        <v>989.16940763212517</v>
+        <v>35</v>
+      </c>
+      <c r="E27">
+        <v>784</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
@@ -1374,17 +1390,17 @@
       <c r="D28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="1">
-        <f>F27*$F$11</f>
-        <v>98682.103784129009</v>
+      <c r="F28" s="2">
+        <f>E27*(1+$G$4)</f>
+        <v>989.16940763212517</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -1393,16 +1409,16 @@
         <v>37</v>
       </c>
       <c r="F29" s="1">
-        <f>F27*$F$12</f>
-        <v>124336.29123423279</v>
+        <f>F28*$F$12</f>
+        <v>98682.103784129009</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -1410,17 +1426,17 @@
       <c r="D30" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="2">
-        <f>F29-F28</f>
-        <v>25654.187450103782</v>
+      <c r="F30" s="1">
+        <f>F28*$F$13</f>
+        <v>124336.29123423279</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -1429,51 +1445,51 @@
         <v>37</v>
       </c>
       <c r="F31" s="2">
-        <f>F25+F30</f>
-        <v>324508.39901005907</v>
+        <f>F30-F29</f>
+        <v>25654.187450103782</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32">
-        <v>830</v>
+        <v>37</v>
+      </c>
+      <c r="F32" s="2">
+        <f>F26+F31</f>
+        <v>324508.39901005907</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="2">
-        <f>E32*(1+$G$4)</f>
-        <v>1047.2074085901324</v>
+        <v>35</v>
+      </c>
+      <c r="E33">
+        <v>830</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -1481,17 +1497,17 @@
       <c r="D34" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="1">
-        <f>F33*$F$11</f>
-        <v>104472.12517962637</v>
+      <c r="F34" s="2">
+        <f>E33*(1+$G$4)</f>
+        <v>1047.2074085901324</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -1500,16 +1516,16 @@
         <v>37</v>
       </c>
       <c r="F35" s="1">
-        <f>F33*$F$12</f>
-        <v>131631.53281175156</v>
+        <f>F34*$F$12</f>
+        <v>104472.12517962637</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -1517,17 +1533,17 @@
       <c r="D36" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="2">
-        <f>F35-F34</f>
-        <v>27159.407632125192</v>
+      <c r="F36" s="1">
+        <f>F34*$F$13</f>
+        <v>131631.53281175156</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
@@ -1536,51 +1552,51 @@
         <v>37</v>
       </c>
       <c r="F37" s="2">
-        <f>F31+F36</f>
-        <v>351667.80664218427</v>
+        <f>F36-F35</f>
+        <v>27159.407632125192</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
         <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38">
-        <v>754</v>
+        <v>37</v>
+      </c>
+      <c r="F38" s="2">
+        <f>F32+F37</f>
+        <v>351667.80664218427</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
-      </c>
-      <c r="F39" s="2">
-        <f>E38*(1+$G$4)</f>
-        <v>951.31853744212037</v>
+        <v>35</v>
+      </c>
+      <c r="E39">
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1588,17 +1604,17 @@
       <c r="D40" t="s">
         <v>37</v>
       </c>
-      <c r="F40" s="1">
-        <f>F39*$F$11</f>
-        <v>94906.00287402203</v>
+      <c r="F40" s="2">
+        <f>E39*(1+$G$4)</f>
+        <v>951.31853744212037</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1607,16 +1623,16 @@
         <v>37</v>
       </c>
       <c r="F41" s="1">
-        <f>F39*$F$12</f>
-        <v>119578.5249880249</v>
+        <f>F40*$F$12</f>
+        <v>94906.00287402203</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
         <v>34</v>
@@ -1624,26 +1640,44 @@
       <c r="D42" t="s">
         <v>37</v>
       </c>
-      <c r="F42" s="2">
-        <f>F41-F40</f>
-        <v>24672.522114002873</v>
+      <c r="F42" s="1">
+        <f>F40*$F$13</f>
+        <v>119578.5249880249</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" s="2">
+        <f>F42-F41</f>
+        <v>24672.522114002873</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>95</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C43" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F43" s="2">
-        <f>F42+F37</f>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="2">
+        <f>F43+F38</f>
         <v>376340.32875618711</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Format Payroll to Revenue Ratio as percentages instead of currency
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B9468C-8018-324A-BE19-F39372D50071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C93C186-DA37-414B-8D27-2BF50BE7DDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1660" windowWidth="25800" windowHeight="17980" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
@@ -745,7 +745,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add new Marketing ROI and Marketing Efficiency metrics to YOY table
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C93C186-DA37-414B-8D27-2BF50BE7DDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903561D3-8057-C04F-8AB8-E0714F58ADAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1660" windowWidth="25800" windowHeight="17980" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="1360" yWindow="1020" windowWidth="28880" windowHeight="18620" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="107">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -332,9 +332,6 @@
     <t>Private Visit Count</t>
   </si>
   <si>
-    <t>AFC / RCM Payments</t>
-  </si>
-  <si>
     <t>Value_2024_Jan_July</t>
   </si>
   <si>
@@ -345,18 +342,35 @@
   </si>
   <si>
     <t>Payroll to Revenue Ratio</t>
+  </si>
+  <si>
+    <t>AFC / Vendor Payments</t>
+  </si>
+  <si>
+    <t>MARKETING_EFFICIENCY</t>
+  </si>
+  <si>
+    <t>MARKETING_ROI</t>
+  </si>
+  <si>
+    <t>Marketing ROI (1$ Earned…)</t>
+  </si>
+  <si>
+    <t>Marketing Efficiency (# of visits per dollar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,6 +387,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,10 +416,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -408,8 +431,12 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -742,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,10 +802,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
         <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -807,7 +834,7 @@
         <v>788324</v>
       </c>
       <c r="G2" s="5">
-        <f t="shared" ref="G2:G11" si="0">(F2-E2)/E2</f>
+        <f t="shared" ref="G2:G13" si="0">(F2-E2)/E2</f>
         <v>-0.12080700834778535</v>
       </c>
       <c r="H2">
@@ -966,11 +993,11 @@
         <v>56914</v>
       </c>
       <c r="F8" s="7">
-        <v>64665.48</v>
+        <v>66195</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0.13619636644762279</v>
+        <v>0.16307059774396457</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -978,233 +1005,255 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="7">
-        <v>70417</v>
-      </c>
-      <c r="F9" s="7">
-        <v>84980</v>
+        <v>17</v>
+      </c>
+      <c r="E9" s="9">
+        <f>((E3-E8)/E8)</f>
+        <v>11.109234986119409</v>
+      </c>
+      <c r="F9" s="9">
+        <f>(F3-F8)/F8</f>
+        <v>14.005106125840321</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0.20681085533322918</v>
+        <v>0.26067241743821234</v>
       </c>
       <c r="H9">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.49</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.39</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="10">
+        <f>E4/E8</f>
+        <v>0.11004322310854975</v>
+      </c>
+      <c r="F10" s="10">
+        <f>F4/F8</f>
+        <v>0.11937457511896669</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>-0.20408163265306117</v>
+        <v>8.4797152853404126E-2</v>
       </c>
       <c r="H10">
-        <v>-20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="7">
+        <v>70417</v>
+      </c>
+      <c r="F11" s="7">
+        <v>84980</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.20681085533322918</v>
+      </c>
+      <c r="H11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E12" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.20408163265306117</v>
+      </c>
+      <c r="H12">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="7">
         <f>108025/E4</f>
         <v>17.24812390228325</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F13" s="7">
         <f>74590/F4</f>
         <v>9.4393824348266264</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>-0.4527299033620073</v>
       </c>
-      <c r="H11">
+      <c r="H13">
         <v>-45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E14" s="4">
         <f>E2/E4</f>
         <v>143.1654159348555</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F14" s="4">
         <f>F2/F4</f>
         <v>99.762591748924322</v>
       </c>
-      <c r="G12" s="5">
-        <f t="shared" ref="G12:G13" si="1">(F12-E12)/E12</f>
+      <c r="G14" s="5">
+        <f t="shared" ref="G14:G15" si="1">(F14-E14)/E14</f>
         <v>-0.30316556482943302</v>
       </c>
-      <c r="H12">
+      <c r="H14">
         <v>-30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E15" s="4">
         <f>E3/E4</f>
         <v>110.04071531215072</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F15" s="4">
         <f>F3/F4</f>
         <v>125.6976714755758</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>0.1422833004948327</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4">
-        <f>E13-E12</f>
-        <v>-33.124700622704779</v>
-      </c>
-      <c r="F14" s="4">
-        <f>F13-F12</f>
-        <v>25.93507972665148</v>
-      </c>
-      <c r="G14" s="5">
-        <f>-1*(F14-E14)/E14</f>
-        <v>1.7829528792442793</v>
-      </c>
-      <c r="H14">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15">
-        <v>685</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="2">
-        <f>E15*(1+$G$4)</f>
-        <v>864.26153600510929</v>
+        <v>9</v>
+      </c>
+      <c r="E16" s="4">
+        <f>E15-E14</f>
+        <v>-33.124700622704779</v>
+      </c>
+      <c r="F16" s="4">
+        <f>F15-F14</f>
+        <v>25.93507972665148</v>
+      </c>
+      <c r="G16" s="5">
+        <f>-1*(F16-E16)/E16</f>
+        <v>1.7829528792442793</v>
+      </c>
+      <c r="H16">
+        <v>1778</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1">
-        <f>F16*$F$12</f>
-        <v>86220.970780775984</v>
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>685</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1212,17 +1261,17 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="1">
-        <f>F16*$F$13</f>
-        <v>108635.66262174676</v>
+      <c r="F18" s="2">
+        <f>E17*(1+$G$4)</f>
+        <v>864.26153600510929</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1230,17 +1279,17 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="2">
-        <f>F18-F17</f>
-        <v>22414.691840970772</v>
+      <c r="F19" s="1">
+        <f>F18*$F$14</f>
+        <v>86220.970780775984</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -1248,34 +1297,35 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="2">
-        <f>250000+F19</f>
-        <v>272414.69184097077</v>
+      <c r="F20" s="1">
+        <f>F18*$F$15</f>
+        <v>108635.66262174676</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21">
-        <v>808</v>
+        <v>37</v>
+      </c>
+      <c r="F21" s="2">
+        <f>F20-F19</f>
+        <v>22414.691840970772</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1284,34 +1334,33 @@
         <v>37</v>
       </c>
       <c r="F22" s="2">
-        <f>E21*(1+$G$4)</f>
-        <v>1019.4501037841289</v>
+        <f>250000+F21</f>
+        <v>272414.69184097077</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="1">
-        <f>F22*$F$12</f>
-        <v>101702.98451221459</v>
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>808</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -1319,17 +1368,17 @@
       <c r="D24" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="1">
-        <f>F22*$F$13</f>
-        <v>128142.5042311991</v>
+      <c r="F24" s="2">
+        <f>E23*(1+$G$4)</f>
+        <v>1019.4501037841289</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1337,17 +1386,17 @@
       <c r="D25" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="2">
-        <f>F24-F23</f>
-        <v>26439.519718984506</v>
+      <c r="F25" s="1">
+        <f>F24*$F$14</f>
+        <v>101702.98451221459</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -1355,34 +1404,35 @@
       <c r="D26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="2">
-        <f>F20+F25</f>
-        <v>298854.21155995526</v>
+      <c r="F26" s="1">
+        <f>F24*$F$15</f>
+        <v>128142.5042311991</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27">
-        <v>784</v>
+        <v>37</v>
+      </c>
+      <c r="F27" s="2">
+        <f>F26-F25</f>
+        <v>26439.519718984506</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
@@ -1391,34 +1441,33 @@
         <v>37</v>
       </c>
       <c r="F28" s="2">
-        <f>E27*(1+$G$4)</f>
-        <v>989.16940763212517</v>
+        <f>F22+F27</f>
+        <v>298854.21155995526</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="1">
-        <f>F28*$F$12</f>
-        <v>98682.103784129009</v>
+        <v>35</v>
+      </c>
+      <c r="E29">
+        <v>784</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -1426,17 +1475,17 @@
       <c r="D30" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="1">
-        <f>F28*$F$13</f>
-        <v>124336.29123423279</v>
+      <c r="F30" s="2">
+        <f>E29*(1+$G$4)</f>
+        <v>989.16940763212517</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -1444,17 +1493,17 @@
       <c r="D31" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="2">
-        <f>F30-F29</f>
-        <v>25654.187450103782</v>
+      <c r="F31" s="1">
+        <f>F30*$F$14</f>
+        <v>98682.103784129009</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
@@ -1462,34 +1511,35 @@
       <c r="D32" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="2">
-        <f>F26+F31</f>
-        <v>324508.39901005907</v>
+      <c r="F32" s="1">
+        <f>F30*$F$15</f>
+        <v>124336.29123423279</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33">
-        <v>830</v>
+        <v>37</v>
+      </c>
+      <c r="F33" s="2">
+        <f>F32-F31</f>
+        <v>25654.187450103782</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -1498,34 +1548,33 @@
         <v>37</v>
       </c>
       <c r="F34" s="2">
-        <f>E33*(1+$G$4)</f>
-        <v>1047.2074085901324</v>
+        <f>F28+F33</f>
+        <v>324508.39901005907</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="1">
-        <f>F34*$F$12</f>
-        <v>104472.12517962637</v>
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>830</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -1533,17 +1582,17 @@
       <c r="D36" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="1">
-        <f>F34*$F$13</f>
-        <v>131631.53281175156</v>
+      <c r="F36" s="2">
+        <f>E35*(1+$G$4)</f>
+        <v>1047.2074085901324</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
@@ -1551,17 +1600,17 @@
       <c r="D37" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="2">
-        <f>F36-F35</f>
-        <v>27159.407632125192</v>
+      <c r="F37" s="1">
+        <f>F36*$F$14</f>
+        <v>104472.12517962637</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>34</v>
@@ -1569,34 +1618,35 @@
       <c r="D38" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="2">
-        <f>F32+F37</f>
-        <v>351667.80664218427</v>
+      <c r="F38" s="1">
+        <f>F36*$F$15</f>
+        <v>131631.53281175156</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39">
-        <v>754</v>
+        <v>37</v>
+      </c>
+      <c r="F39" s="2">
+        <f>F38-F37</f>
+        <v>27159.407632125192</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1605,34 +1655,33 @@
         <v>37</v>
       </c>
       <c r="F40" s="2">
-        <f>E39*(1+$G$4)</f>
-        <v>951.31853744212037</v>
+        <f>F34+F39</f>
+        <v>351667.80664218427</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="1">
-        <f>F40*$F$12</f>
-        <v>94906.00287402203</v>
+        <v>35</v>
+      </c>
+      <c r="E41">
+        <v>754</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
         <v>34</v>
@@ -1640,17 +1689,17 @@
       <c r="D42" t="s">
         <v>37</v>
       </c>
-      <c r="F42" s="1">
-        <f>F40*$F$13</f>
-        <v>119578.5249880249</v>
+      <c r="F42" s="2">
+        <f>E41*(1+$G$4)</f>
+        <v>951.31853744212037</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
         <v>34</v>
@@ -1658,26 +1707,62 @@
       <c r="D43" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="2">
-        <f>F42-F41</f>
-        <v>24672.522114002873</v>
+      <c r="F43" s="1">
+        <f>F42*$F$14</f>
+        <v>94906.00287402203</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="1">
+        <f>F42*$F$15</f>
+        <v>119578.5249880249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="2">
+        <f>F44-F43</f>
+        <v>24672.522114002873</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>95</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F44" s="2">
-        <f>F43+F38</f>
+      <c r="C46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="2">
+        <f>F45+F40</f>
         <v>376340.32875618711</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add two decimal places formatting for small values in YOY table
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903561D3-8057-C04F-8AB8-E0714F58ADAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B37B3C-B858-D44E-B793-EEFD1E03D462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1020" windowWidth="28880" windowHeight="18620" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="4440" yWindow="1020" windowWidth="25800" windowHeight="18620" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,11 +993,11 @@
         <v>56914</v>
       </c>
       <c r="F8" s="7">
-        <v>66195</v>
+        <v>64665</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0.16307059774396457</v>
+        <v>0.13618793267034474</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -1022,11 +1022,11 @@
       </c>
       <c r="F9" s="9">
         <f>(F3-F8)/F8</f>
-        <v>14.005106125840321</v>
+        <v>14.360132993118379</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0.26067241743821234</v>
+        <v>0.29263023161008389</v>
       </c>
       <c r="H9">
         <v>26</v>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="F10" s="10">
         <f>F4/F8</f>
-        <v>0.11937457511896669</v>
+        <v>0.12219902574808629</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>8.4797152853404126E-2</v>
+        <v>0.11046389133427793</v>
       </c>
       <c r="H10">
         <v>9</v>

</xml_diff>

<commit_message>
Update marketing metrics data and ensure decimal formatting
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B37B3C-B858-D44E-B793-EEFD1E03D462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC92F31-E67D-F343-A14F-7329832EE41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1020" windowWidth="25800" windowHeight="18620" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,8 +363,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -421,7 +422,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -433,6 +434,8 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -772,7 +775,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1128,11 +1131,11 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="11">
         <f>108025/E4</f>
         <v>17.24812390228325</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="11">
         <f>74590/F4</f>
         <v>9.4393824348266264</v>
       </c>
@@ -1215,11 +1218,11 @@
       <c r="D16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="12">
         <f>E15-E14</f>
         <v>-33.124700622704779</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="12">
         <f>F15-F14</f>
         <v>25.93507972665148</v>
       </c>

</xml_diff>

<commit_message>
Add group titles and indented metrics to YOY table for better organization
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC92F31-E67D-F343-A14F-7329832EE41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C73E875-3D13-284C-A115-E5230C1E6C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,10 +819,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -831,52 +831,52 @@
         <v>9</v>
       </c>
       <c r="E2" s="6">
-        <v>896645</v>
+        <v>689185</v>
       </c>
       <c r="F2" s="6">
-        <v>788324</v>
+        <v>993263</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G13" si="0">(F2-E2)/E2</f>
-        <v>-0.12080700834778535</v>
+        <v>0.44121389757467155</v>
       </c>
       <c r="H2">
-        <v>-12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6">
-        <v>689185</v>
-      </c>
-      <c r="F3" s="6">
-        <v>993263</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6263</v>
+      </c>
+      <c r="F3" s="3">
+        <v>7902</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="0"/>
-        <v>0.44121389757467155</v>
+        <v>0.26169567300015967</v>
       </c>
       <c r="H3">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -885,44 +885,44 @@
         <v>14</v>
       </c>
       <c r="E4" s="3">
-        <v>6263</v>
+        <v>5036</v>
       </c>
       <c r="F4" s="3">
-        <v>7902</v>
+        <v>6117</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="0"/>
-        <v>0.26169567300015967</v>
+        <v>0.21465448768864179</v>
       </c>
       <c r="H4">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5036</v>
-      </c>
-      <c r="F5" s="3">
-        <v>6117</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>896645</v>
+      </c>
+      <c r="F5" s="6">
+        <v>788324</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21465448768864179</v>
+        <f>(F5-E5)/E5</f>
+        <v>-0.12080700834778535</v>
       </c>
       <c r="H5">
-        <v>22</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1020,11 +1020,11 @@
         <v>17</v>
       </c>
       <c r="E9" s="9">
-        <f>((E3-E8)/E8)</f>
+        <f>((E2-E8)/E8)</f>
         <v>11.109234986119409</v>
       </c>
       <c r="F9" s="9">
-        <f>(F3-F8)/F8</f>
+        <f>(F2-F8)/F8</f>
         <v>14.360132993118379</v>
       </c>
       <c r="G9" s="5">
@@ -1049,11 +1049,11 @@
         <v>17</v>
       </c>
       <c r="E10" s="10">
-        <f>E4/E8</f>
+        <f>E3/E8</f>
         <v>0.11004322310854975</v>
       </c>
       <c r="F10" s="10">
-        <f>F4/F8</f>
+        <f>F3/F8</f>
         <v>0.12219902574808629</v>
       </c>
       <c r="G10" s="5">
@@ -1132,11 +1132,11 @@
         <v>20</v>
       </c>
       <c r="E13" s="11">
-        <f>108025/E4</f>
+        <f>108025/E3</f>
         <v>17.24812390228325</v>
       </c>
       <c r="F13" s="11">
-        <f>74590/F4</f>
+        <f>74590/F3</f>
         <v>9.4393824348266264</v>
       </c>
       <c r="G13" s="5">
@@ -1161,11 +1161,11 @@
         <v>20</v>
       </c>
       <c r="E14" s="4">
-        <f>E2/E4</f>
+        <f>E5/E3</f>
         <v>143.1654159348555</v>
       </c>
       <c r="F14" s="4">
-        <f>F2/F4</f>
+        <f>F5/F3</f>
         <v>99.762591748924322</v>
       </c>
       <c r="G14" s="5">
@@ -1190,11 +1190,11 @@
         <v>14</v>
       </c>
       <c r="E15" s="4">
-        <f>E3/E4</f>
+        <f>E2/E3</f>
         <v>110.04071531215072</v>
       </c>
       <c r="F15" s="4">
-        <f>F3/F4</f>
+        <f>F2/F3</f>
         <v>125.6976714755758</v>
       </c>
       <c r="G15" s="5">
@@ -1234,7 +1234,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1250,8 +1250,9 @@
       <c r="E17">
         <v>685</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1265,11 +1266,11 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <f>E17*(1+$G$4)</f>
+        <f>E17*(1+$G$3)</f>
         <v>864.26153600510929</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>86220.970780775984</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1305,7 +1306,7 @@
         <v>108635.66262174676</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>22414.691840970772</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>272414.69184097077</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1372,11 +1373,11 @@
         <v>37</v>
       </c>
       <c r="F24" s="2">
-        <f>E23*(1+$G$4)</f>
+        <f>E23*(1+$G$3)</f>
         <v>1019.4501037841289</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>101702.98451221459</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>128142.5042311991</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>26439.519718984506</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>298854.21155995526</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1479,11 +1480,11 @@
         <v>37</v>
       </c>
       <c r="F30" s="2">
-        <f>E29*(1+$G$4)</f>
+        <f>E29*(1+$G$3)</f>
         <v>989.16940763212517</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>98682.103784129009</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>37</v>
       </c>
       <c r="F36" s="2">
-        <f>E35*(1+$G$4)</f>
+        <f>E35*(1+$G$3)</f>
         <v>1047.2074085901324</v>
       </c>
     </row>
@@ -1693,7 +1694,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="2">
-        <f>E41*(1+$G$4)</f>
+        <f>E41*(1+$G$3)</f>
         <v>951.31853744212037</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement complete authentication system with login page, JWT tokens, and protected API endpoints
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C73E875-3D13-284C-A115-E5230C1E6C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F52AC-4041-3B45-94E5-2E5182EDA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="300" yWindow="760" windowWidth="28080" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>